<commit_message>
add functions for pft from family and woodiness
</commit_message>
<xml_diff>
--- a/speciesMappingExampleLists/102ae489-04e3-481d-97df-45905837dc1a_Species__PFT.xlsx
+++ b/speciesMappingExampleLists/102ae489-04e3-481d-97df-45905837dc1a_Species__PFT.xlsx
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>not assigned ()</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>not assigned (shrub/tree)</t>
+          <t>not assigned</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>grass</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>grass</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>grass</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>not assigned ()</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>legume</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>forb</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>legume</t>
+          <t>not found</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>grass</t>
+          <t>not found</t>
         </is>
       </c>
     </row>

</xml_diff>